<commit_message>
Ultima corrida y arreglar output paths
</commit_message>
<xml_diff>
--- a/data_management/management/2. harmonization/ENCOVI harmonization/Statistics_for presentation_TS.xlsx
+++ b/data_management/management/2. harmonization/ENCOVI harmonization/Statistics_for presentation_TS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb563583\GitHub\VEN\data_management\management\2. harmonization\ENCOVI harmonization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb550905\Github\VEN\data_management\management\2. harmonization\ENCOVI harmonization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD95CCA-66F4-4C6C-B557-7FDB49077A2A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A2F455-37A5-4B40-A3AD-EA3068B9806C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16890" yWindow="5430" windowWidth="10125" windowHeight="7500" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="8" r:id="rId1"/>
@@ -349,12 +349,6 @@
     <t>Cuenta de ahorro</t>
   </si>
   <si>
-    <t>Tarjeta de credito</t>
-  </si>
-  <si>
-    <t>Tarjeta de debito</t>
-  </si>
-  <si>
     <t>No tiene cuenta o tarjeta</t>
   </si>
   <si>
@@ -668,6 +662,12 @@
   </si>
   <si>
     <t>Propia (pagándose)</t>
+  </si>
+  <si>
+    <t>Tarjeta de débito</t>
+  </si>
+  <si>
+    <t>Tarjeta de crédito</t>
   </si>
 </sst>
 </file>
@@ -2337,7 +2337,7 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Tarjeta de credito</c:v>
+                  <c:v>Tarjeta de crédito</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2390,7 +2390,7 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Tarjeta de debito</c:v>
+                  <c:v>Tarjeta de débito</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2555,23 +2555,10 @@
         <c:axId val="1619460416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.60000000000000009"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2606,6 +2593,7 @@
         <c:crossAx val="1599717888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -14731,13 +14719,13 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="7" width="6.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="2" max="7" width="6.44140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" s="2">
         <v>2014</v>
       </c>
@@ -14757,142 +14745,142 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>131</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="B6" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="B7" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="B8" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="B9" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
         <v>137</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -14909,14 +14897,14 @@
       <selection activeCell="B3" sqref="B3:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -14924,7 +14912,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -14935,7 +14923,7 @@
         <v>3.9381025780518026</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -14946,7 +14934,7 @@
         <v>3.9683259286124462</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -14957,7 +14945,7 @@
         <v>4.0317949647897962</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -14968,7 +14956,7 @@
         <v>3.9864599389488315</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -14979,7 +14967,7 @@
         <v>3.4061716081844837</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -14990,7 +14978,7 @@
         <v>3.675159428174207</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -15001,7 +14989,7 @@
         <v>3.4454619639133197</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -15012,7 +15000,7 @@
         <v>3.566355366155892</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -15023,7 +15011,7 @@
         <v>3.3366579018950042</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -15034,7 +15022,7 @@
         <v>3.3034122162782968</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>63</v>
       </c>
@@ -15045,7 +15033,7 @@
         <v>3.3729259225677759</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -15056,7 +15044,7 @@
         <v>3.3427025720071328</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -15067,7 +15055,7 @@
         <v>2.7110345452896909</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -15078,7 +15066,7 @@
         <v>2.2335056064315291</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -15089,7 +15077,7 @@
         <v>1.3932964608456495</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -15113,18 +15101,18 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
-    <col min="2" max="7" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" style="1" customWidth="1"/>
+    <col min="2" max="7" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -15144,9 +15132,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B4" s="3">
         <v>50.753768844221106</v>
@@ -15167,9 +15155,9 @@
         <v>51.873904370428583</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B5" s="3">
         <v>49.246231155778894</v>
@@ -15190,7 +15178,7 @@
         <v>48.126095629571417</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>69</v>
       </c>
@@ -15213,12 +15201,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>0</v>
       </c>
@@ -15238,9 +15226,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B11" s="3">
         <v>27.603534915959106</v>
@@ -15261,9 +15249,9 @@
         <v>24.511137304681597</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B12" s="3">
         <v>19.026165309305146</v>
@@ -15284,9 +15272,9 @@
         <v>14.745972738537795</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B13" s="3">
         <v>15.49124935019927</v>
@@ -15307,9 +15295,9 @@
         <v>13.274095566234474</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B14" s="3">
         <v>13.411887021313465</v>
@@ -15330,9 +15318,9 @@
         <v>13.026264091637199</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B15" s="3">
         <v>11.349852711835037</v>
@@ -15353,9 +15341,9 @@
         <v>12.690784900414059</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B16" s="3">
         <v>8.7506498007277767</v>
@@ -15376,9 +15364,9 @@
         <v>11.493940218212591</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B17" s="3">
         <v>4.3666608906601976</v>
@@ -15399,7 +15387,7 @@
         <v>10.257805180282286</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>69</v>
       </c>
@@ -15422,12 +15410,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>0</v>
       </c>
@@ -15447,9 +15435,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B23" s="3">
         <v>24.105545617173522</v>
@@ -15470,9 +15458,9 @@
         <v>21.759747102212856</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B24" s="3">
         <v>36.203041144901611</v>
@@ -15493,9 +15481,9 @@
         <v>36.869637212102965</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B25" s="3">
         <v>26.095706618962431</v>
@@ -15516,9 +15504,9 @@
         <v>25.199458076170405</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B26" s="3">
         <v>9.704830053667262</v>
@@ -15539,9 +15527,9 @@
         <v>10.35300316122234</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B27" s="3">
         <v>3.8908765652951698</v>
@@ -15562,7 +15550,7 @@
         <v>5.8181544482914349</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>69</v>
       </c>
@@ -15585,12 +15573,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
         <v>0</v>
       </c>
@@ -15610,7 +15598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>1</v>
       </c>
@@ -15633,7 +15621,7 @@
         <v>4.3197001299839792</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>2</v>
       </c>
@@ -15656,7 +15644,7 @@
         <v>13.209999697711677</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>3</v>
       </c>
@@ -15679,7 +15667,7 @@
         <v>20.730933164051873</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>4</v>
       </c>
@@ -15702,7 +15690,7 @@
         <v>22.901363320334937</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>5</v>
       </c>
@@ -15725,7 +15713,7 @@
         <v>15.734107191439195</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>6</v>
       </c>
@@ -15748,7 +15736,7 @@
         <v>10.555908225265258</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>7</v>
       </c>
@@ -15771,7 +15759,7 @@
         <v>5.1419243674616855</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>8</v>
       </c>
@@ -15794,7 +15782,7 @@
         <v>3.0712493576373143</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>9</v>
       </c>
@@ -15817,7 +15805,7 @@
         <v>1.6323569420513286</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>10</v>
       </c>
@@ -15840,7 +15828,7 @@
         <v>1.299839787189021</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>11</v>
       </c>
@@ -15863,7 +15851,7 @@
         <v>0.69828602521084615</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>12</v>
       </c>
@@ -15886,7 +15874,7 @@
         <v>0.32647138841026574</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>13</v>
       </c>
@@ -15909,7 +15897,7 @@
         <v>0.1571899277530909</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>14</v>
       </c>
@@ -15932,7 +15920,7 @@
         <v>0.12696109549288112</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>15</v>
       </c>
@@ -15955,7 +15943,7 @@
         <v>4.5343248390314679E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>16</v>
       </c>
@@ -15978,7 +15966,7 @@
         <v>4.8366131616335656E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>17</v>
       </c>
@@ -16001,7 +15989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>18</v>
       </c>
@@ -16024,7 +16012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>69</v>
       </c>
@@ -16047,12 +16035,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B55" s="2" t="s">
         <v>0</v>
       </c>
@@ -16072,9 +16060,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B56" s="3">
         <v>1.767457979552937</v>
@@ -16095,9 +16083,9 @@
         <v>4.3189167951159071</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B57" s="3">
         <v>7.6243285392479638</v>
@@ -16118,9 +16106,9 @@
         <v>13.207604195001057</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B58" s="3">
         <v>17.882516028417953</v>
@@ -16141,9 +16129,9 @@
         <v>20.727173814489074</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B59" s="3">
         <v>22.665049384855308</v>
@@ -16164,9 +16152,9 @@
         <v>22.897210384743254</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B60" s="3">
         <v>18.88754115404609</v>
@@ -16187,7 +16175,7 @@
         <v>15.731253966814762</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>6</v>
       </c>
@@ -16210,9 +16198,9 @@
         <v>10.55399401577659</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B62" s="3">
         <v>19.944550337896377</v>
@@ -16233,7 +16221,7 @@
         <v>12.563846828059358</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>69</v>
       </c>
@@ -16256,12 +16244,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B67" s="2" t="s">
         <v>0</v>
       </c>
@@ -16281,7 +16269,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>13</v>
       </c>
@@ -16304,7 +16292,7 @@
         <v>0.81705598066854612</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>14</v>
       </c>
@@ -16327,7 +16315,7 @@
         <v>2.1743858236004834</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>15</v>
       </c>
@@ -16350,7 +16338,7 @@
         <v>2.5164115988723319</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>16</v>
       </c>
@@ -16373,7 +16361,7 @@
         <v>0.34202577527184858</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>17</v>
       </c>
@@ -16396,9 +16384,9 @@
         <v>3.2756745871929116</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -16415,317 +16403,317 @@
       <selection activeCell="H22" sqref="H22:N47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D3">
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B4">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B5">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B6">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B7">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B8">
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B9">
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F9">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B10">
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D10">
         <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F10">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B11">
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D11">
         <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F11">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B12">
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F12" s="8">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B13">
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D13">
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F13">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B14">
         <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D14">
         <v>24</v>
       </c>
       <c r="E14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F14">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F15">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D16" s="8"/>
       <c r="E16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F16">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F17">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F18">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B22">
         <v>2014</v>
       </c>
       <c r="C22" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E22">
         <v>2015</v>
       </c>
       <c r="F22" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H22" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I22" s="2">
         <v>2014</v>
@@ -16746,51 +16734,51 @@
         <v>2019</v>
       </c>
       <c r="P22" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="Q22" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="R22" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B24">
         <v>413</v>
       </c>
       <c r="D24" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E24">
         <v>384</v>
       </c>
       <c r="H24" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M24" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P24" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="Q24">
         <v>654</v>
@@ -16802,31 +16790,31 @@
         <v>1.98</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B25">
         <v>438</v>
       </c>
       <c r="D25" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E25">
         <v>567</v>
       </c>
       <c r="H25" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M25" s="11"/>
       <c r="P25" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="Q25" s="8">
         <v>2304</v>
@@ -16838,38 +16826,38 @@
         <v>8.94</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B26">
         <v>456</v>
       </c>
       <c r="D26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E26">
         <v>451</v>
       </c>
       <c r="H26" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M26" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="Q26" s="8">
         <v>1088</v>
@@ -16882,30 +16870,30 @@
       </c>
       <c r="U26" s="8"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="H27" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J27" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M27" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P27" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="Q27" s="8">
         <v>1711</v>
@@ -16917,42 +16905,42 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B28">
         <v>918</v>
       </c>
       <c r="D28" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E28" s="8">
         <v>1071</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M28" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P28" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="Q28" s="8">
         <v>1594</v>
@@ -16964,38 +16952,38 @@
         <v>22.22</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B29">
         <v>320</v>
       </c>
       <c r="D29" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E29">
         <v>166</v>
       </c>
       <c r="H29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M29" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P29" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="Q29" s="8">
         <v>1985</v>
@@ -17007,30 +16995,30 @@
         <v>28.22</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="H30" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M30" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P30" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="Q30">
         <v>750</v>
@@ -17042,38 +17030,38 @@
         <v>30.48</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B31">
         <v>292</v>
       </c>
       <c r="D31" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E31">
         <v>388</v>
       </c>
       <c r="H31" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M31" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P31" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="Q31">
         <v>843</v>
@@ -17085,36 +17073,36 @@
         <v>33.03</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B32">
         <v>77</v>
       </c>
       <c r="D32" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E32">
         <v>90</v>
       </c>
       <c r="H32" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M32" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P32" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="Q32" s="8">
         <v>1921</v>
@@ -17127,33 +17115,33 @@
       </c>
       <c r="U32" s="8"/>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B33">
         <v>451</v>
       </c>
       <c r="D33" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E33">
         <v>466</v>
       </c>
       <c r="H33" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M33" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P33" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="Q33">
         <v>634</v>
@@ -17165,42 +17153,42 @@
         <v>40.75</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B34">
         <v>390</v>
       </c>
       <c r="D34" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E34">
         <v>354</v>
       </c>
       <c r="H34" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="M34" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="P34" t="s">
         <v>161</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J34" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="L34" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="M34" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="N34" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="P34" t="s">
-        <v>163</v>
       </c>
       <c r="Q34" s="8">
         <v>1001</v>
@@ -17212,40 +17200,40 @@
         <v>43.78</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B35">
         <v>482</v>
       </c>
       <c r="D35" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E35">
         <v>419</v>
       </c>
       <c r="H35" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K35" s="2"/>
       <c r="L35" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M35" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P35" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="Q35">
         <v>909</v>
@@ -17257,42 +17245,42 @@
         <v>46.53</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B36">
         <v>759</v>
       </c>
       <c r="D36" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E36">
         <v>669</v>
       </c>
       <c r="H36" t="s">
+        <v>161</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="M36" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="P36" t="s">
         <v>163</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="M36" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="N36" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="P36" t="s">
-        <v>165</v>
       </c>
       <c r="Q36" s="8">
         <v>1501</v>
@@ -17304,42 +17292,42 @@
         <v>51.06</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B37">
         <v>593</v>
       </c>
       <c r="D37" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E37">
         <v>717</v>
       </c>
       <c r="H37" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M37" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="Q37" s="8">
         <v>2017</v>
@@ -17352,42 +17340,42 @@
       </c>
       <c r="U37" s="8"/>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B38">
         <v>182</v>
       </c>
       <c r="D38" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E38">
         <v>203</v>
       </c>
       <c r="H38" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M38" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P38" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="Q38" s="8">
         <v>2035</v>
@@ -17399,26 +17387,26 @@
         <v>63.31</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="H39" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="11"/>
       <c r="K39" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M39" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N39" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P39" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="Q39" s="8">
         <v>1122</v>
@@ -17430,9 +17418,9 @@
         <v>66.7</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="H40" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="11"/>
@@ -17440,11 +17428,11 @@
       <c r="L40" s="2"/>
       <c r="M40" s="11"/>
       <c r="N40" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Q40" s="8"/>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B41" s="8">
         <v>5771</v>
       </c>
@@ -17452,22 +17440,22 @@
         <v>5945</v>
       </c>
       <c r="H41" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
       <c r="L41" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M41" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P41" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="Q41" s="8">
         <v>2828</v>
@@ -17480,30 +17468,30 @@
       </c>
       <c r="U41" s="8"/>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="H42" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M42" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P42" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="Q42" s="8">
         <v>1613</v>
@@ -17515,30 +17503,30 @@
         <v>80.12</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="H43" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J43" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M43" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P43" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="Q43" s="8">
         <v>2403</v>
@@ -17550,26 +17538,26 @@
         <v>87.38</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="H44" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M44" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P44" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="Q44" s="8">
         <v>1218</v>
@@ -17581,24 +17569,24 @@
         <v>91.07</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="H45" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
       <c r="L45" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M45" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P45" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="Q45" s="8">
         <v>2153</v>
@@ -17610,30 +17598,30 @@
         <v>97.57</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="H46" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M46" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P46" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="Q46">
         <v>803</v>
@@ -17645,30 +17633,30 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="H47" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M47" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="R48" s="8"/>
       <c r="S48" s="8"/>
     </row>
-    <row r="49" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="12:13" x14ac:dyDescent="0.3">
       <c r="L49" t="s">
         <v>69</v>
       </c>
@@ -17683,23 +17671,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="8" customWidth="1"/>
-    <col min="2" max="7" width="9.140625" style="11"/>
-    <col min="8" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="23.5546875" style="8" customWidth="1"/>
+    <col min="2" max="7" width="9.109375" style="11"/>
+    <col min="8" max="16384" width="9.109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
         <v>0</v>
       </c>
@@ -17719,7 +17707,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>72</v>
       </c>
@@ -17742,7 +17730,7 @@
         <v>35.440998791784132</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>73</v>
       </c>
@@ -17765,7 +17753,7 @@
         <v>61.568666935159079</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>74</v>
       </c>
@@ -17788,7 +17776,7 @@
         <v>2.8896496173983084</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>75</v>
       </c>
@@ -17811,7 +17799,7 @@
         <v>0.10068465565847766</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>70</v>
       </c>
@@ -17834,7 +17822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>69</v>
       </c>
@@ -17857,12 +17845,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
         <v>0</v>
       </c>
@@ -17882,7 +17870,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>76</v>
       </c>
@@ -17905,7 +17893,7 @@
         <v>81.655255739025364</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>77</v>
       </c>
@@ -17928,7 +17916,7 @@
         <v>12.857430527587596</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>78</v>
       </c>
@@ -17951,7 +17939,7 @@
         <v>0.84575110753121219</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>79</v>
       </c>
@@ -17974,7 +17962,7 @@
         <v>0.42287555376560609</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>80</v>
       </c>
@@ -17997,7 +17985,7 @@
         <v>0.17116391461941199</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>81</v>
       </c>
@@ -18020,7 +18008,7 @@
         <v>0.92629883205799446</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>82</v>
       </c>
@@ -18043,7 +18031,7 @@
         <v>0.5336286749899315</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>70</v>
       </c>
@@ -18066,7 +18054,7 @@
         <v>2.5875956504228754</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>69</v>
       </c>
@@ -18089,12 +18077,12 @@
         <v>99.999999999999986</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B26" s="11" t="s">
         <v>0</v>
       </c>
@@ -18114,7 +18102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>83</v>
       </c>
@@ -18137,7 +18125,7 @@
         <v>32.551349174385827</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>84</v>
       </c>
@@ -18160,7 +18148,7 @@
         <v>7.6016915022150622</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>85</v>
       </c>
@@ -18183,7 +18171,7 @@
         <v>11.387434554973822</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>86</v>
       </c>
@@ -18206,7 +18194,7 @@
         <v>47.180829641562624</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>87</v>
       </c>
@@ -18229,7 +18217,7 @@
         <v>1.2786951268626663</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>69</v>
       </c>
@@ -18252,12 +18240,12 @@
         <v>100.00000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B36" s="11" t="s">
         <v>0</v>
       </c>
@@ -18277,9 +18265,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B37" s="11">
         <v>14.393420150788211</v>
@@ -18300,9 +18288,9 @@
         <v>4.4301248489730165</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B38" s="11">
         <v>51.884852638793703</v>
@@ -18323,9 +18311,9 @@
         <v>85.370519532823195</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B39" s="11">
         <v>6.2371487320082251</v>
@@ -18346,9 +18334,9 @@
         <v>4.5811518324607325</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B40" s="11">
         <v>0.47978067169294036</v>
@@ -18369,7 +18357,7 @@
         <v>0.52356020942408377</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>88</v>
       </c>
@@ -18392,9 +18380,9 @@
         <v>3.2118405155054366</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B42" s="11">
         <v>0.3427004797806717</v>
@@ -18415,7 +18403,7 @@
         <v>0.48328634716069269</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
         <v>89</v>
       </c>
@@ -18438,7 +18426,7 @@
         <v>1.3995167136528395</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
         <v>69</v>
       </c>
@@ -18461,7 +18449,7 @@
         <v>100.00000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
         <v>22</v>
       </c>
@@ -18472,7 +18460,7 @@
       <c r="F46" s="14"/>
       <c r="G46" s="14"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B48" s="11" t="s">
         <v>0</v>
       </c>
@@ -18492,7 +18480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
         <v>92</v>
       </c>
@@ -18515,7 +18503,7 @@
         <v>72.812405598630548</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
         <v>93</v>
       </c>
@@ -18538,7 +18526,7 @@
         <v>5.0448091833652207</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
         <v>69</v>
       </c>
@@ -18561,7 +18549,7 @@
         <v>10.613231295941999</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B52" s="11">
         <v>14.256339958875945</v>
       </c>
@@ -18581,7 +18569,7 @@
         <v>11.529553922062231</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
         <v>22</v>
       </c>
@@ -18604,7 +18592,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
         <v>23</v>
       </c>
@@ -18627,7 +18615,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
         <v>98</v>
       </c>
@@ -18650,7 +18638,7 @@
         <v>72.812405598630548</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
         <v>90</v>
       </c>
@@ -18673,7 +18661,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
         <v>91</v>
       </c>
@@ -18696,7 +18684,7 @@
         <v>0.13089005235602094</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
         <v>70</v>
       </c>
@@ -18719,7 +18707,7 @@
         <v>99.869109947643977</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="s">
         <v>69</v>
       </c>
@@ -18742,12 +18730,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B64" s="11" t="s">
         <v>0</v>
       </c>
@@ -18767,7 +18755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
         <v>94</v>
       </c>
@@ -18790,7 +18778,7 @@
         <v>93.595166163141997</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
         <v>95</v>
       </c>
@@ -18813,7 +18801,7 @@
         <v>4.1993957703927487</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="8" t="s">
         <v>96</v>
       </c>
@@ -18836,7 +18824,7 @@
         <v>0.74521651560926483</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="8" t="s">
         <v>97</v>
       </c>
@@ -18859,7 +18847,7 @@
         <v>1.4602215508559919</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
         <v>69</v>
       </c>
@@ -18882,12 +18870,12 @@
         <v>100.00000000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B73" s="11" t="s">
         <v>0</v>
       </c>
@@ -18907,9 +18895,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B74" s="11">
         <v>66.506189821182943</v>
@@ -18930,9 +18918,9 @@
         <v>78.523962948046716</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="8" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B75" s="11">
         <v>3.3700137551581841</v>
@@ -18953,9 +18941,9 @@
         <v>0.62424486508256138</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B76" s="11">
         <v>7.1526822558459422</v>
@@ -18976,9 +18964,9 @@
         <v>4.5710833668948858</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B77" s="11">
         <v>5.3645116918844566</v>
@@ -18999,9 +18987,9 @@
         <v>9.28312525171164</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B78" s="11">
         <v>9.9037138927097654</v>
@@ -19022,9 +19010,9 @@
         <v>1.8525976641159889</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B79" s="11">
         <v>3.6451169188445669</v>
@@ -19045,9 +19033,9 @@
         <v>2.4768425291985503</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B80" s="11">
         <v>4.0577716643741404</v>
@@ -19068,7 +19056,7 @@
         <v>2.6681433749496577</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
         <v>69</v>
       </c>
@@ -19091,12 +19079,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B85" s="11" t="s">
         <v>0</v>
       </c>
@@ -19116,7 +19104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="8" t="s">
         <v>26</v>
       </c>
@@ -19136,7 +19124,7 @@
         <v>12.066881547139403</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="8" t="s">
         <v>71</v>
       </c>
@@ -19156,7 +19144,7 @@
         <v>1.1153845904538264</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="8" t="s">
         <v>27</v>
       </c>
@@ -19179,7 +19167,7 @@
         <v>84.35737308622079</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="8" t="s">
         <v>28</v>
       </c>
@@ -19202,7 +19190,7 @@
         <v>55.091515825664885</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="8" t="s">
         <v>29</v>
       </c>
@@ -19225,7 +19213,7 @@
         <v>7.1948998178506374</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="8" t="s">
         <v>30</v>
       </c>
@@ -19248,7 +19236,7 @@
         <v>24.50384771162414</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="8" t="s">
         <v>31</v>
       </c>
@@ -19271,7 +19259,7 @@
         <v>18.844246533751644</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="8" t="s">
         <v>32</v>
       </c>
@@ -19294,7 +19282,7 @@
         <v>87.750781328762983</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="8" t="s">
         <v>33</v>
       </c>
@@ -19317,7 +19305,7 @@
         <v>52.834765032844864</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="8" t="s">
         <v>34</v>
       </c>
@@ -19340,7 +19328,7 @@
         <v>4.5007602635580328</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="8" t="s">
         <v>35</v>
       </c>
@@ -19363,7 +19351,7 @@
         <v>37.131313131313135</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="8" t="s">
         <v>36</v>
       </c>
@@ -19386,7 +19374,7 @@
         <v>47.216619604679302</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="8" t="s">
         <v>37</v>
       </c>
@@ -19409,7 +19397,7 @@
         <v>13.1520420541852</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="8" t="s">
         <v>38</v>
       </c>
@@ -19430,7 +19418,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19444,18 +19432,18 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="7" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -19475,7 +19463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -19498,7 +19486,7 @@
         <v>38.017412555368871</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>93</v>
       </c>
@@ -19521,7 +19509,7 @@
         <v>61.982587444631129</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -19544,12 +19532,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>0</v>
       </c>
@@ -19569,9 +19557,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B11" s="3">
         <v>7.8247847248221634</v>
@@ -19592,9 +19580,9 @@
         <v>1.7227983650305712</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B12" s="3">
         <v>4.0621490078622235</v>
@@ -19615,9 +19603,9 @@
         <v>4.6447995135628144</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B13" s="3">
         <v>28.996630475477346</v>
@@ -19638,9 +19626,9 @@
         <v>32.95611931223187</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B14" s="3">
         <v>38.618494945713216</v>
@@ -19661,9 +19649,9 @@
         <v>40.722224098908896</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B15" s="3">
         <v>5.6158742044178211</v>
@@ -19684,9 +19672,9 @@
         <v>5.9487214133702659</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B16" s="3">
         <v>14.114563833770125</v>
@@ -19707,9 +19695,9 @@
         <v>13.356754383001723</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B17" s="3">
         <v>0.76750280793710224</v>
@@ -19730,7 +19718,7 @@
         <v>0.64858291389386213</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -19753,12 +19741,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>0</v>
       </c>
@@ -19778,9 +19766,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B23" s="3">
         <v>8.1005586592178762</v>
@@ -19801,9 +19789,9 @@
         <v>0.37029200169276344</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B24" s="3">
         <v>0</v>
@@ -19824,9 +19812,9 @@
         <v>0.2010156580617859</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B25" s="3">
         <v>31.6340782122905</v>
@@ -19847,9 +19835,9 @@
         <v>33.273381294964025</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B26" s="3">
         <v>38.896648044692739</v>
@@ -19870,9 +19858,9 @@
         <v>41.007194244604314</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B27" s="3">
         <v>5.516759776536313</v>
@@ -19893,9 +19881,9 @@
         <v>7.5010579771476928</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B28" s="3">
         <v>14.175977653631286</v>
@@ -19916,9 +19904,9 @@
         <v>16.515023275497249</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B29" s="3">
         <v>1.6759776536312849</v>
@@ -19939,7 +19927,7 @@
         <v>1.1320355480321624</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>69</v>
       </c>
@@ -19962,12 +19950,12 @@
         <v>99.999999999999986</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
         <v>0</v>
       </c>
@@ -19987,9 +19975,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B35" s="3">
         <v>29.528535980148884</v>
@@ -20010,9 +19998,9 @@
         <v>43.439823186658629</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B36" s="3">
         <v>1.1166253101736971</v>
@@ -20033,9 +20021,9 @@
         <v>0.98452883263009849</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B37" s="3">
         <v>0</v>
@@ -20056,9 +20044,9 @@
         <v>0.12055455093429776</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B38" s="3">
         <v>0.24813895781637718</v>
@@ -20079,9 +20067,9 @@
         <v>0.76351215591721922</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B39" s="3">
         <v>0.99255583126550873</v>
@@ -20102,9 +20090,9 @@
         <v>1.4868394615230058</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B40" s="3">
         <v>0</v>
@@ -20125,9 +20113,9 @@
         <v>0.64295760498292143</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B41" s="3">
         <v>1.1166253101736971</v>
@@ -20148,9 +20136,9 @@
         <v>1.4064697609001406</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B42" s="3">
         <v>23.325062034739457</v>
@@ -20171,9 +20159,9 @@
         <v>12.999799075748442</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B43" s="3">
         <v>27.915632754342433</v>
@@ -20194,9 +20182,9 @@
         <v>22.121760096443641</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B44" s="3">
         <v>0</v>
@@ -20217,9 +20205,9 @@
         <v>0.24110910186859552</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B45" s="3">
         <v>0.49627791563275436</v>
@@ -20240,9 +20228,9 @@
         <v>0.14064697609001406</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B46" s="3">
         <v>8.4367245657568244</v>
@@ -20263,9 +20251,9 @@
         <v>6.6104078762306617</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B47" s="3">
         <v>1.240694789081886</v>
@@ -20286,9 +20274,9 @@
         <v>2.6120152702431185</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B48" s="3">
         <v>2.2332506203473943</v>
@@ -20309,9 +20297,9 @@
         <v>1.848503114325899</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B49" s="3">
         <v>3.3498759305210917</v>
@@ -20332,7 +20320,7 @@
         <v>4.5810729355033146</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>69</v>
       </c>
@@ -20355,12 +20343,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B54" s="2" t="s">
         <v>0</v>
       </c>
@@ -20380,7 +20368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>43</v>
       </c>
@@ -20403,7 +20391,7 @@
         <v>61.982587444631129</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>44</v>
       </c>
@@ -20422,7 +20410,7 @@
         <v>17.3006993006993</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>45</v>
       </c>
@@ -20441,7 +20429,7 @@
         <v>11.51048951048951</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>46</v>
       </c>
@@ -20460,7 +20448,7 @@
         <v>7.6363636363636367</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>47</v>
       </c>
@@ -20479,7 +20467,7 @@
         <v>5.3286713286713283</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>48</v>
       </c>
@@ -20498,7 +20486,7 @@
         <v>11.692307692307692</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>49</v>
       </c>
@@ -20517,7 +20505,7 @@
         <v>4.335664335664335</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>50</v>
       </c>
@@ -20534,7 +20522,7 @@
         <v>12.88111888111888</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>51</v>
       </c>
@@ -20551,7 +20539,7 @@
         <v>2.6433566433566433</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>52</v>
       </c>
@@ -20580,22 +20568,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="7" width="9.140625" style="2"/>
+    <col min="2" max="7" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -20615,7 +20603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -20624,7 +20612,7 @@
         <v>0.55963780600184299</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -20633,27 +20621,27 @@
         <v>0.40750831363436002</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>210</v>
       </c>
       <c r="G6" s="10">
         <f>5.06430546095597/100</f>
         <v>5.0643054609559701E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>105</v>
+        <v>209</v>
       </c>
       <c r="G7" s="9">
         <f>57.4702512119877/100</f>
         <v>0.574702512119877</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G8" s="9">
         <f>15.2369886614047/100</f>
@@ -20667,6 +20655,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D97C45C73161C540AAAEC0BB7C04B14C" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eaac3f66d04ba47d8e7bacccdec8bc8e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="69ca14ff-5d6d-4eb8-91d9-74d4bb4de445" xmlns:ns4="72d74521-8c27-4702-99f8-167624e069b6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e42dd572579043e93d80e2ef1a203961" ns3:_="" ns4:_="">
     <xsd:import namespace="69ca14ff-5d6d-4eb8-91d9-74d4bb4de445"/>
@@ -20889,22 +20892,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89BB6137-415D-4885-828C-A8FA44D39B10}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="72d74521-8c27-4702-99f8-167624e069b6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="69ca14ff-5d6d-4eb8-91d9-74d4bb4de445"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C30E79AF-C9F7-44BC-84F3-9FDB2966CDCD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDE4FD95-407A-4586-99CF-839F5B5F5351}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20921,29 +20934,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C30E79AF-C9F7-44BC-84F3-9FDB2966CDCD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89BB6137-415D-4885-828C-A8FA44D39B10}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="72d74521-8c27-4702-99f8-167624e069b6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="69ca14ff-5d6d-4eb8-91d9-74d4bb4de445"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>